<commit_message>
predict June 13 | $27,086
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK163"/>
+  <dimension ref="A1:AK164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -18916,6 +18916,119 @@
         <v>32717.048</v>
       </c>
     </row>
+    <row r="164" spans="1:37">
+      <c r="A164" s="2">
+        <v>44724</v>
+      </c>
+      <c r="B164" t="s">
+        <v>37</v>
+      </c>
+      <c r="C164">
+        <v>6</v>
+      </c>
+      <c r="D164">
+        <v>12</v>
+      </c>
+      <c r="E164">
+        <v>28395.9</v>
+      </c>
+      <c r="F164">
+        <v>28500.8</v>
+      </c>
+      <c r="G164">
+        <v>26506.5</v>
+      </c>
+      <c r="H164">
+        <v>26569.6</v>
+      </c>
+      <c r="I164">
+        <v>3666.64664503</v>
+      </c>
+      <c r="J164">
+        <v>26457</v>
+      </c>
+      <c r="K164">
+        <v>29056.2</v>
+      </c>
+      <c r="L164">
+        <v>29411.7</v>
+      </c>
+      <c r="M164">
+        <v>28095.9</v>
+      </c>
+      <c r="N164">
+        <v>28380.2</v>
+      </c>
+      <c r="O164">
+        <v>2317.67808556</v>
+      </c>
+      <c r="P164">
+        <v>22690</v>
+      </c>
+      <c r="Q164">
+        <v>-0.03420607406274823</v>
+      </c>
+      <c r="R164">
+        <v>-0.03020021366675896</v>
+      </c>
+      <c r="S164">
+        <v>-0.02597659229265181</v>
+      </c>
+      <c r="T164">
+        <v>-0.02322155643282198</v>
+      </c>
+      <c r="U164">
+        <v>-0.4675954365238278</v>
+      </c>
+      <c r="V164">
+        <v>-0.07353721775346045</v>
+      </c>
+      <c r="W164">
+        <v>30220.14285714286</v>
+      </c>
+      <c r="X164">
+        <v>30734.25714285714</v>
+      </c>
+      <c r="Y164">
+        <v>29325.34285714286</v>
+      </c>
+      <c r="Z164">
+        <v>30009.1</v>
+      </c>
+      <c r="AA164">
+        <v>3085.743094415714</v>
+      </c>
+      <c r="AB164">
+        <v>21806.71428571429</v>
+      </c>
+      <c r="AC164">
+        <v>-0.001356944595448075</v>
+      </c>
+      <c r="AD164">
+        <v>-0.001279945099828333</v>
+      </c>
+      <c r="AE164">
+        <v>-0.001838485249030218</v>
+      </c>
+      <c r="AF164">
+        <v>-0.002706386297454661</v>
+      </c>
+      <c r="AG164">
+        <v>0.4591310232430822</v>
+      </c>
+      <c r="AH164">
+        <v>0.1349148301979546</v>
+      </c>
+      <c r="AI164">
+        <v>29954.45555555556</v>
+      </c>
+      <c r="AJ164">
+        <v>29887.955</v>
+      </c>
+      <c r="AK164">
+        <v>32490.334</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict June 14 | $23,581
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK164"/>
+  <dimension ref="A1:AK165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -19029,6 +19029,119 @@
         <v>32490.334</v>
       </c>
     </row>
+    <row r="165" spans="1:37">
+      <c r="A165" s="2">
+        <v>44725</v>
+      </c>
+      <c r="B165" t="s">
+        <v>37</v>
+      </c>
+      <c r="C165">
+        <v>6</v>
+      </c>
+      <c r="D165">
+        <v>13</v>
+      </c>
+      <c r="E165">
+        <v>26542.2</v>
+      </c>
+      <c r="F165">
+        <v>26853.2</v>
+      </c>
+      <c r="G165">
+        <v>21930.4</v>
+      </c>
+      <c r="H165">
+        <v>22460.1</v>
+      </c>
+      <c r="I165">
+        <v>17333.48812069</v>
+      </c>
+      <c r="J165">
+        <v>85068</v>
+      </c>
+      <c r="K165">
+        <v>28395.9</v>
+      </c>
+      <c r="L165">
+        <v>28500.8</v>
+      </c>
+      <c r="M165">
+        <v>26506.5</v>
+      </c>
+      <c r="N165">
+        <v>26569.6</v>
+      </c>
+      <c r="O165">
+        <v>3666.64664503</v>
+      </c>
+      <c r="P165">
+        <v>26457</v>
+      </c>
+      <c r="Q165">
+        <v>-0.02272492617754551</v>
+      </c>
+      <c r="R165">
+        <v>-0.03097066813546989</v>
+      </c>
+      <c r="S165">
+        <v>-0.05657053164340708</v>
+      </c>
+      <c r="T165">
+        <v>-0.06379800001409441</v>
+      </c>
+      <c r="U165">
+        <v>0.5820344800576827</v>
+      </c>
+      <c r="V165">
+        <v>0.1660202732481268</v>
+      </c>
+      <c r="W165">
+        <v>30012.3</v>
+      </c>
+      <c r="X165">
+        <v>30496.88571428572</v>
+      </c>
+      <c r="Y165">
+        <v>28895.7</v>
+      </c>
+      <c r="Z165">
+        <v>29532.24285714286</v>
+      </c>
+      <c r="AA165">
+        <v>3471.898166584286</v>
+      </c>
+      <c r="AB165">
+        <v>23987.71428571429</v>
+      </c>
+      <c r="AC165">
+        <v>-0.002699712927610367</v>
+      </c>
+      <c r="AD165">
+        <v>-0.002312063626062828</v>
+      </c>
+      <c r="AE165">
+        <v>-0.006502133502181207</v>
+      </c>
+      <c r="AF165">
+        <v>-0.006859432379878009</v>
+      </c>
+      <c r="AG165">
+        <v>0.4899321801048339</v>
+      </c>
+      <c r="AH165">
+        <v>0.1846748964079853</v>
+      </c>
+      <c r="AI165">
+        <v>29609.25555555556</v>
+      </c>
+      <c r="AJ165">
+        <v>29762.935</v>
+      </c>
+      <c r="AK165">
+        <v>32233.014</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict June 15 | $22,211
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK165"/>
+  <dimension ref="A1:AK166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -19142,6 +19142,119 @@
         <v>32233.014</v>
       </c>
     </row>
+    <row r="166" spans="1:37">
+      <c r="A166" s="2">
+        <v>44726</v>
+      </c>
+      <c r="B166" t="s">
+        <v>37</v>
+      </c>
+      <c r="C166">
+        <v>6</v>
+      </c>
+      <c r="D166">
+        <v>14</v>
+      </c>
+      <c r="E166">
+        <v>22460</v>
+      </c>
+      <c r="F166">
+        <v>23309</v>
+      </c>
+      <c r="G166">
+        <v>20824</v>
+      </c>
+      <c r="H166">
+        <v>22111</v>
+      </c>
+      <c r="I166">
+        <v>10473.22068889</v>
+      </c>
+      <c r="J166">
+        <v>59767</v>
+      </c>
+      <c r="K166">
+        <v>26542.2</v>
+      </c>
+      <c r="L166">
+        <v>26853.2</v>
+      </c>
+      <c r="M166">
+        <v>21930.4</v>
+      </c>
+      <c r="N166">
+        <v>22460.1</v>
+      </c>
+      <c r="O166">
+        <v>17333.48812069</v>
+      </c>
+      <c r="P166">
+        <v>85068</v>
+      </c>
+      <c r="Q166">
+        <v>-0.0652805510654707</v>
+      </c>
+      <c r="R166">
+        <v>-0.05780890360972324</v>
+      </c>
+      <c r="S166">
+        <v>-0.1726406730424612</v>
+      </c>
+      <c r="T166">
+        <v>-0.1546692460556426</v>
+      </c>
+      <c r="U166">
+        <v>3.727340755397001</v>
+      </c>
+      <c r="V166">
+        <v>2.215330536341989</v>
+      </c>
+      <c r="W166">
+        <v>29531.52857142857</v>
+      </c>
+      <c r="X166">
+        <v>29800.82857142857</v>
+      </c>
+      <c r="Y166">
+        <v>27759.77142857143</v>
+      </c>
+      <c r="Z166">
+        <v>28261.35714285714</v>
+      </c>
+      <c r="AA166">
+        <v>5455.616051517142</v>
+      </c>
+      <c r="AB166">
+        <v>33068.14285714286</v>
+      </c>
+      <c r="AC166">
+        <v>-0.006785662894661188</v>
+      </c>
+      <c r="AD166">
+        <v>-0.007727948569006922</v>
+      </c>
+      <c r="AE166">
+        <v>-0.01489360543970798</v>
+      </c>
+      <c r="AF166">
+        <v>-0.01624909641634948</v>
+      </c>
+      <c r="AG166">
+        <v>0.5402141384415096</v>
+      </c>
+      <c r="AH166">
+        <v>0.1980119293084626</v>
+      </c>
+      <c r="AI166">
+        <v>28788.15555555555</v>
+      </c>
+      <c r="AJ166">
+        <v>29404.35</v>
+      </c>
+      <c r="AK166">
+        <v>31892.858</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict June 16 | $22,172
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK166"/>
+  <dimension ref="A1:AK167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -19255,6 +19255,119 @@
         <v>31892.858</v>
       </c>
     </row>
+    <row r="167" spans="1:37">
+      <c r="A167" s="2">
+        <v>44727</v>
+      </c>
+      <c r="B167" t="s">
+        <v>37</v>
+      </c>
+      <c r="C167">
+        <v>6</v>
+      </c>
+      <c r="D167">
+        <v>15</v>
+      </c>
+      <c r="E167">
+        <v>22115</v>
+      </c>
+      <c r="F167">
+        <v>22773.3</v>
+      </c>
+      <c r="G167">
+        <v>20089</v>
+      </c>
+      <c r="H167">
+        <v>22559.6</v>
+      </c>
+      <c r="I167">
+        <v>14784.40560659</v>
+      </c>
+      <c r="J167">
+        <v>67896</v>
+      </c>
+      <c r="K167">
+        <v>22460</v>
+      </c>
+      <c r="L167">
+        <v>23309</v>
+      </c>
+      <c r="M167">
+        <v>20824</v>
+      </c>
+      <c r="N167">
+        <v>22111</v>
+      </c>
+      <c r="O167">
+        <v>10473.22068889</v>
+      </c>
+      <c r="P167">
+        <v>59767</v>
+      </c>
+      <c r="Q167">
+        <v>-0.1538003631952137</v>
+      </c>
+      <c r="R167">
+        <v>-0.1319842700311322</v>
+      </c>
+      <c r="S167">
+        <v>-0.05045051617845553</v>
+      </c>
+      <c r="T167">
+        <v>-0.01554311868602543</v>
+      </c>
+      <c r="U167">
+        <v>-0.39578112518572</v>
+      </c>
+      <c r="V167">
+        <v>-0.2974208868199558</v>
+      </c>
+      <c r="W167">
+        <v>28261.08571428571</v>
+      </c>
+      <c r="X167">
+        <v>28623.54285714286</v>
+      </c>
+      <c r="Y167">
+        <v>26563.17142857143</v>
+      </c>
+      <c r="Z167">
+        <v>26977.41428571429</v>
+      </c>
+      <c r="AA167">
+        <v>6130.560395318572</v>
+      </c>
+      <c r="AB167">
+        <v>36981.71428571428</v>
+      </c>
+      <c r="AC167">
+        <v>-0.01638328398615215</v>
+      </c>
+      <c r="AD167">
+        <v>-0.02339009403222276</v>
+      </c>
+      <c r="AE167">
+        <v>-0.04133731169134258</v>
+      </c>
+      <c r="AF167">
+        <v>-0.04526458766909237</v>
+      </c>
+      <c r="AG167">
+        <v>0.704429223321055</v>
+      </c>
+      <c r="AH167">
+        <v>0.3828012654717061</v>
+      </c>
+      <c r="AI167">
+        <v>27921.86666666667</v>
+      </c>
+      <c r="AJ167">
+        <v>29033.885</v>
+      </c>
+      <c r="AK167">
+        <v>31526.308</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict June 17 | $21,013
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK167"/>
+  <dimension ref="A1:AK168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -19368,6 +19368,119 @@
         <v>31526.308</v>
       </c>
     </row>
+    <row r="168" spans="1:37">
+      <c r="A168" s="2">
+        <v>44728</v>
+      </c>
+      <c r="B168" t="s">
+        <v>37</v>
+      </c>
+      <c r="C168">
+        <v>6</v>
+      </c>
+      <c r="D168">
+        <v>16</v>
+      </c>
+      <c r="E168">
+        <v>22557</v>
+      </c>
+      <c r="F168">
+        <v>22950</v>
+      </c>
+      <c r="G168">
+        <v>20200</v>
+      </c>
+      <c r="H168">
+        <v>20366.3</v>
+      </c>
+      <c r="I168">
+        <v>7892.29096304</v>
+      </c>
+      <c r="J168">
+        <v>39183</v>
+      </c>
+      <c r="K168">
+        <v>22115</v>
+      </c>
+      <c r="L168">
+        <v>22773.3</v>
+      </c>
+      <c r="M168">
+        <v>20089</v>
+      </c>
+      <c r="N168">
+        <v>22559.6</v>
+      </c>
+      <c r="O168">
+        <v>14784.40560659</v>
+      </c>
+      <c r="P168">
+        <v>67896</v>
+      </c>
+      <c r="Q168">
+        <v>-0.01536064113980407</v>
+      </c>
+      <c r="R168">
+        <v>-0.02298253893345925</v>
+      </c>
+      <c r="S168">
+        <v>-0.03529581252401071</v>
+      </c>
+      <c r="T168">
+        <v>0.02028854416353854</v>
+      </c>
+      <c r="U168">
+        <v>0.4116388879567208</v>
+      </c>
+      <c r="V168">
+        <v>0.1360115113691502</v>
+      </c>
+      <c r="W168">
+        <v>26977.91428571428</v>
+      </c>
+      <c r="X168">
+        <v>27405.94285714285</v>
+      </c>
+      <c r="Y168">
+        <v>25169.02857142857</v>
+      </c>
+      <c r="Z168">
+        <v>25887.24285714285</v>
+      </c>
+      <c r="AA168">
+        <v>7838.385838248571</v>
+      </c>
+      <c r="AB168">
+        <v>43430</v>
+      </c>
+      <c r="AC168">
+        <v>-0.04525936394240394</v>
+      </c>
+      <c r="AD168">
+        <v>-0.04145428085070774</v>
+      </c>
+      <c r="AE168">
+        <v>-0.0452855081360752</v>
+      </c>
+      <c r="AF168">
+        <v>-0.04631096974703715</v>
+      </c>
+      <c r="AG168">
+        <v>0.5525333347219146</v>
+      </c>
+      <c r="AH168">
+        <v>0.268123375472283</v>
+      </c>
+      <c r="AI168">
+        <v>26944.45555555555</v>
+      </c>
+      <c r="AJ168">
+        <v>28702.52</v>
+      </c>
+      <c r="AK168">
+        <v>31215.066</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict June 18 | $20,618
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK168"/>
+  <dimension ref="A1:AK169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -19481,6 +19481,119 @@
         <v>31215.066</v>
       </c>
     </row>
+    <row r="169" spans="1:37">
+      <c r="A169" s="2">
+        <v>44729</v>
+      </c>
+      <c r="B169" t="s">
+        <v>37</v>
+      </c>
+      <c r="C169">
+        <v>6</v>
+      </c>
+      <c r="D169">
+        <v>17</v>
+      </c>
+      <c r="E169">
+        <v>20366.3</v>
+      </c>
+      <c r="F169">
+        <v>21327.2</v>
+      </c>
+      <c r="G169">
+        <v>20231.3</v>
+      </c>
+      <c r="H169">
+        <v>20432.9</v>
+      </c>
+      <c r="I169">
+        <v>6404.16986731</v>
+      </c>
+      <c r="J169">
+        <v>32072</v>
+      </c>
+      <c r="K169">
+        <v>22557</v>
+      </c>
+      <c r="L169">
+        <v>22950</v>
+      </c>
+      <c r="M169">
+        <v>20200</v>
+      </c>
+      <c r="N169">
+        <v>20366.3</v>
+      </c>
+      <c r="O169">
+        <v>7892.29096304</v>
+      </c>
+      <c r="P169">
+        <v>39183</v>
+      </c>
+      <c r="Q169">
+        <v>0.0199864345466878</v>
+      </c>
+      <c r="R169">
+        <v>0.007759086298428475</v>
+      </c>
+      <c r="S169">
+        <v>0.005525411916969425</v>
+      </c>
+      <c r="T169">
+        <v>-0.0972224684834837</v>
+      </c>
+      <c r="U169">
+        <v>-0.4661746185100543</v>
+      </c>
+      <c r="V169">
+        <v>-0.4228967833156593</v>
+      </c>
+      <c r="W169">
+        <v>25887.37142857143</v>
+      </c>
+      <c r="X169">
+        <v>26303.65714285714</v>
+      </c>
+      <c r="Y169">
+        <v>23784.42857142857</v>
+      </c>
+      <c r="Z169">
+        <v>24500.24285714286</v>
+      </c>
+      <c r="AA169">
+        <v>8688.708202792857</v>
+      </c>
+      <c r="AB169">
+        <v>46507.42857142857</v>
+      </c>
+      <c r="AC169">
+        <v>-0.04628775948369875</v>
+      </c>
+      <c r="AD169">
+        <v>-0.04358966279931829</v>
+      </c>
+      <c r="AE169">
+        <v>-0.05349702129040593</v>
+      </c>
+      <c r="AF169">
+        <v>-0.03924245991276709</v>
+      </c>
+      <c r="AG169">
+        <v>0.6838777332700117</v>
+      </c>
+      <c r="AH169">
+        <v>0.3299800269261061</v>
+      </c>
+      <c r="AI169">
+        <v>25751.97777777778</v>
+      </c>
+      <c r="AJ169">
+        <v>28291.835</v>
+      </c>
+      <c r="AK169">
+        <v>30837.394</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict June 19 | $19,130
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK169"/>
+  <dimension ref="A1:AK170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -19594,6 +19594,119 @@
         <v>30837.394</v>
       </c>
     </row>
+    <row r="170" spans="1:37">
+      <c r="A170" s="2">
+        <v>44730</v>
+      </c>
+      <c r="B170" t="s">
+        <v>37</v>
+      </c>
+      <c r="C170">
+        <v>6</v>
+      </c>
+      <c r="D170">
+        <v>18</v>
+      </c>
+      <c r="E170">
+        <v>20440.3</v>
+      </c>
+      <c r="F170">
+        <v>20740.1</v>
+      </c>
+      <c r="G170">
+        <v>17600</v>
+      </c>
+      <c r="H170">
+        <v>18950</v>
+      </c>
+      <c r="I170">
+        <v>13006.20331051</v>
+      </c>
+      <c r="J170">
+        <v>63068</v>
+      </c>
+      <c r="K170">
+        <v>20366.3</v>
+      </c>
+      <c r="L170">
+        <v>21327.2</v>
+      </c>
+      <c r="M170">
+        <v>20231.3</v>
+      </c>
+      <c r="N170">
+        <v>20432.9</v>
+      </c>
+      <c r="O170">
+        <v>6404.16986731</v>
+      </c>
+      <c r="P170">
+        <v>32072</v>
+      </c>
+      <c r="Q170">
+        <v>-0.09711841113623265</v>
+      </c>
+      <c r="R170">
+        <v>-0.0707102396514161</v>
+      </c>
+      <c r="S170">
+        <v>0.001549504950494995</v>
+      </c>
+      <c r="T170">
+        <v>0.003270107972484171</v>
+      </c>
+      <c r="U170">
+        <v>-0.1885537548854885</v>
+      </c>
+      <c r="V170">
+        <v>-0.1814817650511702</v>
+      </c>
+      <c r="W170">
+        <v>24498.94285714286</v>
+      </c>
+      <c r="X170">
+        <v>25017.88571428572</v>
+      </c>
+      <c r="Y170">
+        <v>22553.87142857143</v>
+      </c>
+      <c r="Z170">
+        <v>23268.52857142857</v>
+      </c>
+      <c r="AA170">
+        <v>8981.699996730002</v>
+      </c>
+      <c r="AB170">
+        <v>47590.42857142857</v>
+      </c>
+      <c r="AC170">
+        <v>-0.03926865187279184</v>
+      </c>
+      <c r="AD170">
+        <v>-0.03960321865408632</v>
+      </c>
+      <c r="AE170">
+        <v>-0.05291922476468656</v>
+      </c>
+      <c r="AF170">
+        <v>-0.05258485987515468</v>
+      </c>
+      <c r="AG170">
+        <v>0.6621935349385291</v>
+      </c>
+      <c r="AH170">
+        <v>0.3016867737234787</v>
+      </c>
+      <c r="AI170">
+        <v>24667.76666666667</v>
+      </c>
+      <c r="AJ170">
+        <v>27862.48</v>
+      </c>
+      <c r="AK170">
+        <v>30450.996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict June 20 | $20,051
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK170"/>
+  <dimension ref="A1:AK171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -19707,6 +19707,119 @@
         <v>30450.996</v>
       </c>
     </row>
+    <row r="171" spans="1:37">
+      <c r="A171" s="2">
+        <v>44731</v>
+      </c>
+      <c r="B171" t="s">
+        <v>37</v>
+      </c>
+      <c r="C171">
+        <v>6</v>
+      </c>
+      <c r="D171">
+        <v>19</v>
+      </c>
+      <c r="E171">
+        <v>18950</v>
+      </c>
+      <c r="F171">
+        <v>20799.9</v>
+      </c>
+      <c r="G171">
+        <v>17911</v>
+      </c>
+      <c r="H171">
+        <v>20555.5</v>
+      </c>
+      <c r="I171">
+        <v>9585.68835663</v>
+      </c>
+      <c r="J171">
+        <v>45499</v>
+      </c>
+      <c r="K171">
+        <v>20440.3</v>
+      </c>
+      <c r="L171">
+        <v>20740.1</v>
+      </c>
+      <c r="M171">
+        <v>17600</v>
+      </c>
+      <c r="N171">
+        <v>18950</v>
+      </c>
+      <c r="O171">
+        <v>13006.20331051</v>
+      </c>
+      <c r="P171">
+        <v>63068</v>
+      </c>
+      <c r="Q171">
+        <v>0.003633453302759992</v>
+      </c>
+      <c r="R171">
+        <v>-0.02752822686522383</v>
+      </c>
+      <c r="S171">
+        <v>-0.1300608463123971</v>
+      </c>
+      <c r="T171">
+        <v>-0.07257413289351988</v>
+      </c>
+      <c r="U171">
+        <v>1.03089605366341</v>
+      </c>
+      <c r="V171">
+        <v>0.9664504864055874</v>
+      </c>
+      <c r="W171">
+        <v>23268.1</v>
+      </c>
+      <c r="X171">
+        <v>23779.08571428572</v>
+      </c>
+      <c r="Y171">
+        <v>21054.45714285714</v>
+      </c>
+      <c r="Z171">
+        <v>21921.35714285714</v>
+      </c>
+      <c r="AA171">
+        <v>10508.63217172286</v>
+      </c>
+      <c r="AB171">
+        <v>53358.71428571428</v>
+      </c>
+      <c r="AC171">
+        <v>-0.05264350460433244</v>
+      </c>
+      <c r="AD171">
+        <v>-0.04812824967564731</v>
+      </c>
+      <c r="AE171">
+        <v>-0.04769417268764599</v>
+      </c>
+      <c r="AF171">
+        <v>-0.04727081964800649</v>
+      </c>
+      <c r="AG171">
+        <v>0.4575584554723305</v>
+      </c>
+      <c r="AH171">
+        <v>0.2202893811455741</v>
+      </c>
+      <c r="AI171">
+        <v>23431.62222222222</v>
+      </c>
+      <c r="AJ171">
+        <v>27337.46</v>
+      </c>
+      <c r="AK171">
+        <v>30058.006</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict June 21 | $20,501
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK171"/>
+  <dimension ref="A1:AK172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -19820,6 +19820,119 @@
         <v>30058.006</v>
       </c>
     </row>
+    <row r="172" spans="1:37">
+      <c r="A172" s="2">
+        <v>44732</v>
+      </c>
+      <c r="B172" t="s">
+        <v>37</v>
+      </c>
+      <c r="C172">
+        <v>6</v>
+      </c>
+      <c r="D172">
+        <v>20</v>
+      </c>
+      <c r="E172">
+        <v>20550.1</v>
+      </c>
+      <c r="F172">
+        <v>21038.3</v>
+      </c>
+      <c r="G172">
+        <v>19625</v>
+      </c>
+      <c r="H172">
+        <v>20550</v>
+      </c>
+      <c r="I172">
+        <v>7167.6102756</v>
+      </c>
+      <c r="J172">
+        <v>37760</v>
+      </c>
+      <c r="K172">
+        <v>18950</v>
+      </c>
+      <c r="L172">
+        <v>20799.9</v>
+      </c>
+      <c r="M172">
+        <v>17911</v>
+      </c>
+      <c r="N172">
+        <v>20555.5</v>
+      </c>
+      <c r="O172">
+        <v>9585.68835663</v>
+      </c>
+      <c r="P172">
+        <v>45499</v>
+      </c>
+      <c r="Q172">
+        <v>-0.07290988879810956</v>
+      </c>
+      <c r="R172">
+        <v>0.00288330335919329</v>
+      </c>
+      <c r="S172">
+        <v>0.01767045454545446</v>
+      </c>
+      <c r="T172">
+        <v>0.08472295514511874</v>
+      </c>
+      <c r="U172">
+        <v>-0.2629910414452743</v>
+      </c>
+      <c r="V172">
+        <v>-0.2785723346229466</v>
+      </c>
+      <c r="W172">
+        <v>21918.68571428571</v>
+      </c>
+      <c r="X172">
+        <v>22678.95714285714</v>
+      </c>
+      <c r="Y172">
+        <v>19826.52857142857</v>
+      </c>
+      <c r="Z172">
+        <v>21062.2</v>
+      </c>
+      <c r="AA172">
+        <v>11354.20955909429</v>
+      </c>
+      <c r="AB172">
+        <v>56079</v>
+      </c>
+      <c r="AC172">
+        <v>-0.04723785783783126</v>
+      </c>
+      <c r="AD172">
+        <v>-0.04774653727542801</v>
+      </c>
+      <c r="AE172">
+        <v>-0.06256335183332389</v>
+      </c>
+      <c r="AF172">
+        <v>-0.05432118771382047</v>
+      </c>
+      <c r="AG172">
+        <v>0.6716286683562215</v>
+      </c>
+      <c r="AH172">
+        <v>0.3688590531682953</v>
+      </c>
+      <c r="AI172">
+        <v>22487.24444444444</v>
+      </c>
+      <c r="AJ172">
+        <v>26779.65</v>
+      </c>
+      <c r="AK172">
+        <v>29715.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict June 22 | $20,902
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK172"/>
+  <dimension ref="A1:AK173"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -19933,6 +19933,119 @@
         <v>29715.9</v>
       </c>
     </row>
+    <row r="173" spans="1:37">
+      <c r="A173" s="2">
+        <v>44733</v>
+      </c>
+      <c r="B173" t="s">
+        <v>37</v>
+      </c>
+      <c r="C173">
+        <v>6</v>
+      </c>
+      <c r="D173">
+        <v>21</v>
+      </c>
+      <c r="E173">
+        <v>20551.2</v>
+      </c>
+      <c r="F173">
+        <v>21698.9</v>
+      </c>
+      <c r="G173">
+        <v>20323.6</v>
+      </c>
+      <c r="H173">
+        <v>20701.9</v>
+      </c>
+      <c r="I173">
+        <v>5232.17356545</v>
+      </c>
+      <c r="J173">
+        <v>33111</v>
+      </c>
+      <c r="K173">
+        <v>20550.1</v>
+      </c>
+      <c r="L173">
+        <v>21038.3</v>
+      </c>
+      <c r="M173">
+        <v>19625</v>
+      </c>
+      <c r="N173">
+        <v>20550</v>
+      </c>
+      <c r="O173">
+        <v>7167.6102756</v>
+      </c>
+      <c r="P173">
+        <v>37760</v>
+      </c>
+      <c r="Q173">
+        <v>0.08443799472295499</v>
+      </c>
+      <c r="R173">
+        <v>0.01146159356535348</v>
+      </c>
+      <c r="S173">
+        <v>0.09569538272569922</v>
+      </c>
+      <c r="T173">
+        <v>-0.000267568290725162</v>
+      </c>
+      <c r="U173">
+        <v>-0.2522592004941953</v>
+      </c>
+      <c r="V173">
+        <v>-0.1700916503659421</v>
+      </c>
+      <c r="W173">
+        <v>21062.67142857143</v>
+      </c>
+      <c r="X173">
+        <v>21848.25714285714</v>
+      </c>
+      <c r="Y173">
+        <v>19497.18571428571</v>
+      </c>
+      <c r="Z173">
+        <v>20789.32857142857</v>
+      </c>
+      <c r="AA173">
+        <v>9901.94129551</v>
+      </c>
+      <c r="AB173">
+        <v>49320.71428571428</v>
+      </c>
+      <c r="AC173">
+        <v>-0.05440713821219756</v>
+      </c>
+      <c r="AD173">
+        <v>-0.04291025563333327</v>
+      </c>
+      <c r="AE173">
+        <v>-0.05195749666348653</v>
+      </c>
+      <c r="AF173">
+        <v>-0.03310390840536145</v>
+      </c>
+      <c r="AG173">
+        <v>0.550910736712942</v>
+      </c>
+      <c r="AH173">
+        <v>0.3053458234724276</v>
+      </c>
+      <c r="AI173">
+        <v>21617.22222222222</v>
+      </c>
+      <c r="AJ173">
+        <v>26218.105</v>
+      </c>
+      <c r="AK173">
+        <v>29357.418</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict June 23 | $20,160
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK173"/>
+  <dimension ref="A1:AK174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -20046,6 +20046,119 @@
         <v>29357.418</v>
       </c>
     </row>
+    <row r="174" spans="1:37">
+      <c r="A174" s="2">
+        <v>44734</v>
+      </c>
+      <c r="B174" t="s">
+        <v>37</v>
+      </c>
+      <c r="C174">
+        <v>6</v>
+      </c>
+      <c r="D174">
+        <v>22</v>
+      </c>
+      <c r="E174">
+        <v>20704.1</v>
+      </c>
+      <c r="F174">
+        <v>20860.1</v>
+      </c>
+      <c r="G174">
+        <v>19750</v>
+      </c>
+      <c r="H174">
+        <v>19951.3</v>
+      </c>
+      <c r="I174">
+        <v>6091.94667736</v>
+      </c>
+      <c r="J174">
+        <v>33996</v>
+      </c>
+      <c r="K174">
+        <v>20551.2</v>
+      </c>
+      <c r="L174">
+        <v>21698.9</v>
+      </c>
+      <c r="M174">
+        <v>20323.6</v>
+      </c>
+      <c r="N174">
+        <v>20701.9</v>
+      </c>
+      <c r="O174">
+        <v>5232.17356545</v>
+      </c>
+      <c r="P174">
+        <v>33111</v>
+      </c>
+      <c r="Q174">
+        <v>5.352772005995377E-05</v>
+      </c>
+      <c r="R174">
+        <v>0.03139987546522316</v>
+      </c>
+      <c r="S174">
+        <v>0.03559745222929922</v>
+      </c>
+      <c r="T174">
+        <v>0.007391727493917255</v>
+      </c>
+      <c r="U174">
+        <v>-0.2700253830399539</v>
+      </c>
+      <c r="V174">
+        <v>-0.1231197033898305</v>
+      </c>
+      <c r="W174">
+        <v>20789.98571428571</v>
+      </c>
+      <c r="X174">
+        <v>21618.24285714286</v>
+      </c>
+      <c r="Y174">
+        <v>19425.7</v>
+      </c>
+      <c r="Z174">
+        <v>20588.02857142857</v>
+      </c>
+      <c r="AA174">
+        <v>9153.220277875715</v>
+      </c>
+      <c r="AB174">
+        <v>45512.71428571428</v>
+      </c>
+      <c r="AC174">
+        <v>-0.03301877452813674</v>
+      </c>
+      <c r="AD174">
+        <v>-0.03301447032260802</v>
+      </c>
+      <c r="AE174">
+        <v>-0.01362377441089218</v>
+      </c>
+      <c r="AF174">
+        <v>-0.0110465258675161</v>
+      </c>
+      <c r="AG174">
+        <v>-0.01760354270008599</v>
+      </c>
+      <c r="AH174">
+        <v>-0.03542877462870535</v>
+      </c>
+      <c r="AI174">
+        <v>20965.25555555556</v>
+      </c>
+      <c r="AJ174">
+        <v>25763.7</v>
+      </c>
+      <c r="AK174">
+        <v>29001.458</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict Jine 24 | $20,868
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK174"/>
+  <dimension ref="A1:AK175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -20159,6 +20159,119 @@
         <v>29001.458</v>
       </c>
     </row>
+    <row r="175" spans="1:37">
+      <c r="A175" s="2">
+        <v>44735</v>
+      </c>
+      <c r="B175" t="s">
+        <v>37</v>
+      </c>
+      <c r="C175">
+        <v>6</v>
+      </c>
+      <c r="D175">
+        <v>23</v>
+      </c>
+      <c r="E175">
+        <v>19951.3</v>
+      </c>
+      <c r="F175">
+        <v>21200</v>
+      </c>
+      <c r="G175">
+        <v>19880.4</v>
+      </c>
+      <c r="H175">
+        <v>21086.7</v>
+      </c>
+      <c r="I175">
+        <v>3813.63775847</v>
+      </c>
+      <c r="J175">
+        <v>26182</v>
+      </c>
+      <c r="K175">
+        <v>20704.1</v>
+      </c>
+      <c r="L175">
+        <v>20860.1</v>
+      </c>
+      <c r="M175">
+        <v>19750</v>
+      </c>
+      <c r="N175">
+        <v>19951.3</v>
+      </c>
+      <c r="O175">
+        <v>6091.94667736</v>
+      </c>
+      <c r="P175">
+        <v>33996</v>
+      </c>
+      <c r="Q175">
+        <v>0.007439954844485897</v>
+      </c>
+      <c r="R175">
+        <v>-0.03865633741802588</v>
+      </c>
+      <c r="S175">
+        <v>-0.02822334625755274</v>
+      </c>
+      <c r="T175">
+        <v>-0.03625754157830929</v>
+      </c>
+      <c r="U175">
+        <v>0.1643242719598226</v>
+      </c>
+      <c r="V175">
+        <v>0.02672827761166974</v>
+      </c>
+      <c r="W175">
+        <v>20588.42857142857</v>
+      </c>
+      <c r="X175">
+        <v>21344.92857142857</v>
+      </c>
+      <c r="Y175">
+        <v>19377.27142857143</v>
+      </c>
+      <c r="Z175">
+        <v>20215.41428571428</v>
+      </c>
+      <c r="AA175">
+        <v>7911.440430842857</v>
+      </c>
+      <c r="AB175">
+        <v>40669.85714285714</v>
+      </c>
+      <c r="AC175">
+        <v>-0.01103964725452622</v>
+      </c>
+      <c r="AD175">
+        <v>-0.009673878108842968</v>
+      </c>
+      <c r="AE175">
+        <v>-0.001331207495498643</v>
+      </c>
+      <c r="AF175">
+        <v>-0.007770119270381436</v>
+      </c>
+      <c r="AG175">
+        <v>0.0003615633207377313</v>
+      </c>
+      <c r="AH175">
+        <v>-0.01052860556725888</v>
+      </c>
+      <c r="AI175">
+        <v>20686.5</v>
+      </c>
+      <c r="AJ175">
+        <v>25239.915</v>
+      </c>
+      <c r="AK175">
+        <v>28645.926</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict June 25 | $21,219
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK175"/>
+  <dimension ref="A1:AK176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -20272,6 +20272,119 @@
         <v>28645.926</v>
       </c>
     </row>
+    <row r="176" spans="1:37">
+      <c r="A176" s="2">
+        <v>44736</v>
+      </c>
+      <c r="B176" t="s">
+        <v>37</v>
+      </c>
+      <c r="C176">
+        <v>6</v>
+      </c>
+      <c r="D176">
+        <v>24</v>
+      </c>
+      <c r="E176">
+        <v>21090.8</v>
+      </c>
+      <c r="F176">
+        <v>21534.5</v>
+      </c>
+      <c r="G176">
+        <v>20731.1</v>
+      </c>
+      <c r="H176">
+        <v>21210.7</v>
+      </c>
+      <c r="I176">
+        <v>4922.5405392</v>
+      </c>
+      <c r="J176">
+        <v>29149</v>
+      </c>
+      <c r="K176">
+        <v>19951.3</v>
+      </c>
+      <c r="L176">
+        <v>21200</v>
+      </c>
+      <c r="M176">
+        <v>19880.4</v>
+      </c>
+      <c r="N176">
+        <v>21086.7</v>
+      </c>
+      <c r="O176">
+        <v>3813.63775847</v>
+      </c>
+      <c r="P176">
+        <v>26182</v>
+      </c>
+      <c r="Q176">
+        <v>-0.03635994802961728</v>
+      </c>
+      <c r="R176">
+        <v>0.01629426512816345</v>
+      </c>
+      <c r="S176">
+        <v>0.006602531645569787</v>
+      </c>
+      <c r="T176">
+        <v>0.05690857237373015</v>
+      </c>
+      <c r="U176">
+        <v>-0.3739870093343177</v>
+      </c>
+      <c r="V176">
+        <v>-0.2298505706553712</v>
+      </c>
+      <c r="W176">
+        <v>20216.18571428571</v>
+      </c>
+      <c r="X176">
+        <v>21094.92857142857</v>
+      </c>
+      <c r="Y176">
+        <v>19331.61428571428</v>
+      </c>
+      <c r="Z176">
+        <v>20318.32857142857</v>
+      </c>
+      <c r="AA176">
+        <v>7328.775687332857</v>
+      </c>
+      <c r="AB176">
+        <v>38812.57142857143</v>
+      </c>
+      <c r="AC176">
+        <v>-0.007782419256770511</v>
+      </c>
+      <c r="AD176">
+        <v>-0.01191299217806677</v>
+      </c>
+      <c r="AE176">
+        <v>-0.0003208551717189336</v>
+      </c>
+      <c r="AF176">
+        <v>-0.01584813151921684</v>
+      </c>
+      <c r="AG176">
+        <v>-0.03496909610739058</v>
+      </c>
+      <c r="AH176">
+        <v>-0.02614049610404181</v>
+      </c>
+      <c r="AI176">
+        <v>20572.68888888889</v>
+      </c>
+      <c r="AJ176">
+        <v>24810.43</v>
+      </c>
+      <c r="AK176">
+        <v>28274.004</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict June 26 | $21, 406
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK176"/>
+  <dimension ref="A1:AK177"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -20385,6 +20385,119 @@
         <v>28274.004</v>
       </c>
     </row>
+    <row r="177" spans="1:37">
+      <c r="A177" s="2">
+        <v>44737</v>
+      </c>
+      <c r="B177" t="s">
+        <v>37</v>
+      </c>
+      <c r="C177">
+        <v>6</v>
+      </c>
+      <c r="D177">
+        <v>25</v>
+      </c>
+      <c r="E177">
+        <v>21221.6</v>
+      </c>
+      <c r="F177">
+        <v>21589</v>
+      </c>
+      <c r="G177">
+        <v>20888.8</v>
+      </c>
+      <c r="H177">
+        <v>21474.5</v>
+      </c>
+      <c r="I177">
+        <v>1835.57069102</v>
+      </c>
+      <c r="J177">
+        <v>18990</v>
+      </c>
+      <c r="K177">
+        <v>21090.8</v>
+      </c>
+      <c r="L177">
+        <v>21534.5</v>
+      </c>
+      <c r="M177">
+        <v>20731.1</v>
+      </c>
+      <c r="N177">
+        <v>21210.7</v>
+      </c>
+      <c r="O177">
+        <v>4922.5405392</v>
+      </c>
+      <c r="P177">
+        <v>29149</v>
+      </c>
+      <c r="Q177">
+        <v>0.05711407276718816</v>
+      </c>
+      <c r="R177">
+        <v>0.01577830188679252</v>
+      </c>
+      <c r="S177">
+        <v>0.04279088951932541</v>
+      </c>
+      <c r="T177">
+        <v>0.005880483906917533</v>
+      </c>
+      <c r="U177">
+        <v>0.2907729708379232</v>
+      </c>
+      <c r="V177">
+        <v>0.1133221297074325</v>
+      </c>
+      <c r="W177">
+        <v>20319.68571428571</v>
+      </c>
+      <c r="X177">
+        <v>21124.54285714286</v>
+      </c>
+      <c r="Y177">
+        <v>19403.01428571429</v>
+      </c>
+      <c r="Z177">
+        <v>20429.44285714286</v>
+      </c>
+      <c r="AA177">
+        <v>7117.114354745713</v>
+      </c>
+      <c r="AB177">
+        <v>38395</v>
+      </c>
+      <c r="AC177">
+        <v>-0.01583190248195695</v>
+      </c>
+      <c r="AD177">
+        <v>-0.01069368091667606</v>
+      </c>
+      <c r="AE177">
+        <v>-0.0001669809247760247</v>
+      </c>
+      <c r="AF177">
+        <v>0.006170588603242282</v>
+      </c>
+      <c r="AG177">
+        <v>-0.02179943765371393</v>
+      </c>
+      <c r="AH177">
+        <v>0.001437534275999353</v>
+      </c>
+      <c r="AI177">
+        <v>20422.81111111111</v>
+      </c>
+      <c r="AJ177">
+        <v>24378.465</v>
+      </c>
+      <c r="AK177">
+        <v>27967.366</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict June 27 | $21,233
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK177"/>
+  <dimension ref="A1:AK178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -20498,6 +20498,119 @@
         <v>27967.366</v>
       </c>
     </row>
+    <row r="178" spans="1:37">
+      <c r="A178" s="2">
+        <v>44738</v>
+      </c>
+      <c r="B178" t="s">
+        <v>37</v>
+      </c>
+      <c r="C178">
+        <v>6</v>
+      </c>
+      <c r="D178">
+        <v>26</v>
+      </c>
+      <c r="E178">
+        <v>21476.8</v>
+      </c>
+      <c r="F178">
+        <v>21867</v>
+      </c>
+      <c r="G178">
+        <v>20957</v>
+      </c>
+      <c r="H178">
+        <v>21023.3</v>
+      </c>
+      <c r="I178">
+        <v>1913.1909771</v>
+      </c>
+      <c r="J178">
+        <v>20649</v>
+      </c>
+      <c r="K178">
+        <v>21221.6</v>
+      </c>
+      <c r="L178">
+        <v>21589</v>
+      </c>
+      <c r="M178">
+        <v>20888.8</v>
+      </c>
+      <c r="N178">
+        <v>21474.5</v>
+      </c>
+      <c r="O178">
+        <v>1835.57069102</v>
+      </c>
+      <c r="P178">
+        <v>18990</v>
+      </c>
+      <c r="Q178">
+        <v>0.006201756215980403</v>
+      </c>
+      <c r="R178">
+        <v>0.002530822633448615</v>
+      </c>
+      <c r="S178">
+        <v>0.007606928720617745</v>
+      </c>
+      <c r="T178">
+        <v>0.01243711900125866</v>
+      </c>
+      <c r="U178">
+        <v>-0.6271090758110216</v>
+      </c>
+      <c r="V178">
+        <v>-0.3485196747744348</v>
+      </c>
+      <c r="W178">
+        <v>20431.3</v>
+      </c>
+      <c r="X178">
+        <v>21245.81428571429</v>
+      </c>
+      <c r="Y178">
+        <v>19872.84285714286</v>
+      </c>
+      <c r="Z178">
+        <v>20790.08571428572</v>
+      </c>
+      <c r="AA178">
+        <v>5521.309694818571</v>
+      </c>
+      <c r="AB178">
+        <v>32098.14285714286</v>
+      </c>
+      <c r="AC178">
+        <v>0.006201309504246022</v>
+      </c>
+      <c r="AD178">
+        <v>0.001661825017353743</v>
+      </c>
+      <c r="AE178">
+        <v>0.005724645442199749</v>
+      </c>
+      <c r="AF178">
+        <v>0.006543499451018476</v>
+      </c>
+      <c r="AG178">
+        <v>0.04667580887820203</v>
+      </c>
+      <c r="AH178">
+        <v>0.04355237638437116</v>
+      </c>
+      <c r="AI178">
+        <v>20545.94444444445</v>
+      </c>
+      <c r="AJ178">
+        <v>23956.81</v>
+      </c>
+      <c r="AK178">
+        <v>27676.508</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict June 28 | $20,876
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK178"/>
+  <dimension ref="A1:AK179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -20611,6 +20611,119 @@
         <v>27676.508</v>
       </c>
     </row>
+    <row r="179" spans="1:37">
+      <c r="A179" s="2">
+        <v>44739</v>
+      </c>
+      <c r="B179" t="s">
+        <v>37</v>
+      </c>
+      <c r="C179">
+        <v>6</v>
+      </c>
+      <c r="D179">
+        <v>27</v>
+      </c>
+      <c r="E179">
+        <v>21023.4</v>
+      </c>
+      <c r="F179">
+        <v>21528.7</v>
+      </c>
+      <c r="G179">
+        <v>20505.5</v>
+      </c>
+      <c r="H179">
+        <v>20716.3</v>
+      </c>
+      <c r="I179">
+        <v>3973.83637693</v>
+      </c>
+      <c r="J179">
+        <v>22966</v>
+      </c>
+      <c r="K179">
+        <v>21476.8</v>
+      </c>
+      <c r="L179">
+        <v>21867</v>
+      </c>
+      <c r="M179">
+        <v>20957</v>
+      </c>
+      <c r="N179">
+        <v>21023.3</v>
+      </c>
+      <c r="O179">
+        <v>1913.1909771</v>
+      </c>
+      <c r="P179">
+        <v>20649</v>
+      </c>
+      <c r="Q179">
+        <v>0.01202548346967247</v>
+      </c>
+      <c r="R179">
+        <v>0.01287692806521834</v>
+      </c>
+      <c r="S179">
+        <v>0.003264907510244663</v>
+      </c>
+      <c r="T179">
+        <v>-0.02101096649514544</v>
+      </c>
+      <c r="U179">
+        <v>0.04228673210992917</v>
+      </c>
+      <c r="V179">
+        <v>0.08736176935229079</v>
+      </c>
+      <c r="W179">
+        <v>20792.27142857143</v>
+      </c>
+      <c r="X179">
+        <v>21398.25714285714</v>
+      </c>
+      <c r="Y179">
+        <v>20307.98571428571</v>
+      </c>
+      <c r="Z179">
+        <v>20856.91428571428</v>
+      </c>
+      <c r="AA179">
+        <v>4425.2386406</v>
+      </c>
+      <c r="AB179">
+        <v>28548.14285714286</v>
+      </c>
+      <c r="AC179">
+        <v>0.006568209920420366</v>
+      </c>
+      <c r="AD179">
+        <v>0.00595597494573552</v>
+      </c>
+      <c r="AE179">
+        <v>0.02539147044691616</v>
+      </c>
+      <c r="AF179">
+        <v>0.01868796400741541</v>
+      </c>
+      <c r="AG179">
+        <v>-0.1901820667610024</v>
+      </c>
+      <c r="AH179">
+        <v>-0.1443005037842034</v>
+      </c>
+      <c r="AI179">
+        <v>20611.54444444444</v>
+      </c>
+      <c r="AJ179">
+        <v>23440.16</v>
+      </c>
+      <c r="AK179">
+        <v>27387.714</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict June 29 | $20,478
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK179"/>
+  <dimension ref="A1:AK180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -20724,6 +20724,119 @@
         <v>27387.714</v>
       </c>
     </row>
+    <row r="180" spans="1:37">
+      <c r="A180" s="2">
+        <v>44740</v>
+      </c>
+      <c r="B180" t="s">
+        <v>37</v>
+      </c>
+      <c r="C180">
+        <v>6</v>
+      </c>
+      <c r="D180">
+        <v>28</v>
+      </c>
+      <c r="E180">
+        <v>20716.3</v>
+      </c>
+      <c r="F180">
+        <v>21188.5</v>
+      </c>
+      <c r="G180">
+        <v>20165.3</v>
+      </c>
+      <c r="H180">
+        <v>20251.6</v>
+      </c>
+      <c r="I180">
+        <v>3250.53358914</v>
+      </c>
+      <c r="J180">
+        <v>23648</v>
+      </c>
+      <c r="K180">
+        <v>21023.4</v>
+      </c>
+      <c r="L180">
+        <v>21528.7</v>
+      </c>
+      <c r="M180">
+        <v>20505.5</v>
+      </c>
+      <c r="N180">
+        <v>20716.3</v>
+      </c>
+      <c r="O180">
+        <v>3973.83637693</v>
+      </c>
+      <c r="P180">
+        <v>22966</v>
+      </c>
+      <c r="Q180">
+        <v>-0.02111115249944118</v>
+      </c>
+      <c r="R180">
+        <v>-0.01547080074998852</v>
+      </c>
+      <c r="S180">
+        <v>-0.02154411413847401</v>
+      </c>
+      <c r="T180">
+        <v>-0.01460284541437362</v>
+      </c>
+      <c r="U180">
+        <v>1.077072505826632</v>
+      </c>
+      <c r="V180">
+        <v>0.1122088236718486</v>
+      </c>
+      <c r="W180">
+        <v>20859.88571428571</v>
+      </c>
+      <c r="X180">
+        <v>21468.31428571429</v>
+      </c>
+      <c r="Y180">
+        <v>20433.77142857143</v>
+      </c>
+      <c r="Z180">
+        <v>20880.67142857143</v>
+      </c>
+      <c r="AA180">
+        <v>3968.985226504285</v>
+      </c>
+      <c r="AB180">
+        <v>26434.71428571429</v>
+      </c>
+      <c r="AC180">
+        <v>0.01870183453010351</v>
+      </c>
+      <c r="AD180">
+        <v>0.007383635618024813</v>
+      </c>
+      <c r="AE180">
+        <v>0.0233335351561719</v>
+      </c>
+      <c r="AF180">
+        <v>0.003583118058806242</v>
+      </c>
+      <c r="AG180">
+        <v>-0.1465709562531162</v>
+      </c>
+      <c r="AH180">
+        <v>-0.09202420321631237</v>
+      </c>
+      <c r="AI180">
+        <v>20807.8</v>
+      </c>
+      <c r="AJ180">
+        <v>22921.045</v>
+      </c>
+      <c r="AK180">
+        <v>27121.556</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict June 30 | $20,132
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK180"/>
+  <dimension ref="A1:AK181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -20837,6 +20837,119 @@
         <v>27121.556</v>
       </c>
     </row>
+    <row r="181" spans="1:37">
+      <c r="A181" s="2">
+        <v>44741</v>
+      </c>
+      <c r="B181" t="s">
+        <v>37</v>
+      </c>
+      <c r="C181">
+        <v>6</v>
+      </c>
+      <c r="D181">
+        <v>29</v>
+      </c>
+      <c r="E181">
+        <v>20252.5</v>
+      </c>
+      <c r="F181">
+        <v>20397</v>
+      </c>
+      <c r="G181">
+        <v>19828.7</v>
+      </c>
+      <c r="H181">
+        <v>20086.2</v>
+      </c>
+      <c r="I181">
+        <v>4367.31908309</v>
+      </c>
+      <c r="J181">
+        <v>26340</v>
+      </c>
+      <c r="K181">
+        <v>20716.3</v>
+      </c>
+      <c r="L181">
+        <v>21188.5</v>
+      </c>
+      <c r="M181">
+        <v>20165.3</v>
+      </c>
+      <c r="N181">
+        <v>20251.6</v>
+      </c>
+      <c r="O181">
+        <v>3250.53358914</v>
+      </c>
+      <c r="P181">
+        <v>23648</v>
+      </c>
+      <c r="Q181">
+        <v>-0.01460753255895819</v>
+      </c>
+      <c r="R181">
+        <v>-0.01580216176545735</v>
+      </c>
+      <c r="S181">
+        <v>-0.01659067079564025</v>
+      </c>
+      <c r="T181">
+        <v>-0.02243161182257458</v>
+      </c>
+      <c r="U181">
+        <v>-0.1820162480743079</v>
+      </c>
+      <c r="V181">
+        <v>0.02969607245493333</v>
+      </c>
+      <c r="W181">
+        <v>20883.47142857143</v>
+      </c>
+      <c r="X181">
+        <v>21395.4</v>
+      </c>
+      <c r="Y181">
+        <v>20411.15714285714</v>
+      </c>
+      <c r="Z181">
+        <v>20816.34285714286</v>
+      </c>
+      <c r="AA181">
+        <v>3685.893801317143</v>
+      </c>
+      <c r="AB181">
+        <v>25082.85714285714</v>
+      </c>
+      <c r="AC181">
+        <v>0.003623384926904061</v>
+      </c>
+      <c r="AD181">
+        <v>0.003536150715833099</v>
+      </c>
+      <c r="AE181">
+        <v>0.006585035604147154</v>
+      </c>
+      <c r="AF181">
+        <v>0.001535221326856462</v>
+      </c>
+      <c r="AG181">
+        <v>0.04333357322128768</v>
+      </c>
+      <c r="AH181">
+        <v>-0.05169556406805657</v>
+      </c>
+      <c r="AI181">
+        <v>20774.03333333333</v>
+      </c>
+      <c r="AJ181">
+        <v>22424.085</v>
+      </c>
+      <c r="AK181">
+        <v>26925.078</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict July 1 | $19,732
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK181"/>
+  <dimension ref="A1:AK182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -20950,6 +20950,119 @@
         <v>26925.078</v>
       </c>
     </row>
+    <row r="182" spans="1:37">
+      <c r="A182" s="2">
+        <v>44742</v>
+      </c>
+      <c r="B182" t="s">
+        <v>37</v>
+      </c>
+      <c r="C182">
+        <v>6</v>
+      </c>
+      <c r="D182">
+        <v>30</v>
+      </c>
+      <c r="E182">
+        <v>20094</v>
+      </c>
+      <c r="F182">
+        <v>20139.8</v>
+      </c>
+      <c r="G182">
+        <v>18617.5</v>
+      </c>
+      <c r="H182">
+        <v>19949.9</v>
+      </c>
+      <c r="I182">
+        <v>5391.52746356</v>
+      </c>
+      <c r="J182">
+        <v>32136</v>
+      </c>
+      <c r="K182">
+        <v>20252.5</v>
+      </c>
+      <c r="L182">
+        <v>20397</v>
+      </c>
+      <c r="M182">
+        <v>19828.7</v>
+      </c>
+      <c r="N182">
+        <v>20086.2</v>
+      </c>
+      <c r="O182">
+        <v>4367.31908309</v>
+      </c>
+      <c r="P182">
+        <v>26340</v>
+      </c>
+      <c r="Q182">
+        <v>-0.02238816777127184</v>
+      </c>
+      <c r="R182">
+        <v>-0.03735516907756564</v>
+      </c>
+      <c r="S182">
+        <v>-0.01669204028702764</v>
+      </c>
+      <c r="T182">
+        <v>-0.0081672559205197</v>
+      </c>
+      <c r="U182">
+        <v>0.3435698980872461</v>
+      </c>
+      <c r="V182">
+        <v>0.1138362652232747</v>
+      </c>
+      <c r="W182">
+        <v>20818.95714285714</v>
+      </c>
+      <c r="X182">
+        <v>21329.24285714286</v>
+      </c>
+      <c r="Y182">
+        <v>20422.4</v>
+      </c>
+      <c r="Z182">
+        <v>20835.61428571428</v>
+      </c>
+      <c r="AA182">
+        <v>3439.518430707143</v>
+      </c>
+      <c r="AB182">
+        <v>23989.14285714286</v>
+      </c>
+      <c r="AC182">
+        <v>0.001528947744187183</v>
+      </c>
+      <c r="AD182">
+        <v>-0.003206997459978402</v>
+      </c>
+      <c r="AE182">
+        <v>-0.0008704105422727704</v>
+      </c>
+      <c r="AF182">
+        <v>-0.002725255718356658</v>
+      </c>
+      <c r="AG182">
+        <v>0.05590630678780854</v>
+      </c>
+      <c r="AH182">
+        <v>-0.02986473894737602</v>
+      </c>
+      <c r="AI182">
+        <v>20722.5</v>
+      </c>
+      <c r="AJ182">
+        <v>21924.63</v>
+      </c>
+      <c r="AK182">
+        <v>26706.804</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict July 2nd | $19,582
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK182"/>
+  <dimension ref="A1:AK183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -21063,6 +21063,119 @@
         <v>26706.804</v>
       </c>
     </row>
+    <row r="183" spans="1:37">
+      <c r="A183" s="2">
+        <v>44743</v>
+      </c>
+      <c r="B183" t="s">
+        <v>37</v>
+      </c>
+      <c r="C183">
+        <v>7</v>
+      </c>
+      <c r="D183">
+        <v>1</v>
+      </c>
+      <c r="E183">
+        <v>19949.8</v>
+      </c>
+      <c r="F183">
+        <v>20878.3</v>
+      </c>
+      <c r="G183">
+        <v>18950</v>
+      </c>
+      <c r="H183">
+        <v>19245.3</v>
+      </c>
+      <c r="I183">
+        <v>5953.60277338</v>
+      </c>
+      <c r="J183">
+        <v>32011</v>
+      </c>
+      <c r="K183">
+        <v>20094</v>
+      </c>
+      <c r="L183">
+        <v>20139.8</v>
+      </c>
+      <c r="M183">
+        <v>18617.5</v>
+      </c>
+      <c r="N183">
+        <v>19949.9</v>
+      </c>
+      <c r="O183">
+        <v>5391.52746356</v>
+      </c>
+      <c r="P183">
+        <v>32136</v>
+      </c>
+      <c r="Q183">
+        <v>-0.007826194297000377</v>
+      </c>
+      <c r="R183">
+        <v>-0.012609697504535</v>
+      </c>
+      <c r="S183">
+        <v>-0.06108317741455571</v>
+      </c>
+      <c r="T183">
+        <v>-0.006785753402833716</v>
+      </c>
+      <c r="U183">
+        <v>0.2345164987911401</v>
+      </c>
+      <c r="V183">
+        <v>0.2200455580865603</v>
+      </c>
+      <c r="W183">
+        <v>20839.34285714286</v>
+      </c>
+      <c r="X183">
+        <v>21177.78571428571</v>
+      </c>
+      <c r="Y183">
+        <v>20241.98571428571</v>
+      </c>
+      <c r="Z183">
+        <v>20673.21428571429</v>
+      </c>
+      <c r="AA183">
+        <v>3664.93124572</v>
+      </c>
+      <c r="AB183">
+        <v>24839.71428571429</v>
+      </c>
+      <c r="AC183">
+        <v>-0.002732212629492494</v>
+      </c>
+      <c r="AD183">
+        <v>-0.003021116268484083</v>
+      </c>
+      <c r="AE183">
+        <v>0.0007769188820879577</v>
+      </c>
+      <c r="AF183">
+        <v>0.001287642232756141</v>
+      </c>
+      <c r="AG183">
+        <v>0.08151282480601189</v>
+      </c>
+      <c r="AH183">
+        <v>-0.01742074071714674</v>
+      </c>
+      <c r="AI183">
+        <v>20638.94444444445</v>
+      </c>
+      <c r="AJ183">
+        <v>21469.38</v>
+      </c>
+      <c r="AK183">
+        <v>26525.92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
predict July 3 | 19201
</commit_message>
<xml_diff>
--- a/data/btc_df_viz_2022.xlsx
+++ b/data/btc_df_viz_2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="38">
   <si>
     <t>year</t>
   </si>
@@ -491,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK183"/>
+  <dimension ref="A1:AK184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -21176,6 +21176,119 @@
         <v>26525.92</v>
       </c>
     </row>
+    <row r="184" spans="1:37">
+      <c r="A184" s="2">
+        <v>44744</v>
+      </c>
+      <c r="B184" t="s">
+        <v>37</v>
+      </c>
+      <c r="C184">
+        <v>7</v>
+      </c>
+      <c r="D184">
+        <v>2</v>
+      </c>
+      <c r="E184">
+        <v>19250.8</v>
+      </c>
+      <c r="F184">
+        <v>19430.4</v>
+      </c>
+      <c r="G184">
+        <v>18969.6</v>
+      </c>
+      <c r="H184">
+        <v>19226.9</v>
+      </c>
+      <c r="I184">
+        <v>1293.38922751</v>
+      </c>
+      <c r="J184">
+        <v>15723</v>
+      </c>
+      <c r="K184">
+        <v>19949.8</v>
+      </c>
+      <c r="L184">
+        <v>20878.3</v>
+      </c>
+      <c r="M184">
+        <v>18950</v>
+      </c>
+      <c r="N184">
+        <v>19245.3</v>
+      </c>
+      <c r="O184">
+        <v>5953.60277338</v>
+      </c>
+      <c r="P184">
+        <v>32011</v>
+      </c>
+      <c r="Q184">
+        <v>-0.00717627152383804</v>
+      </c>
+      <c r="R184">
+        <v>0.0366686858856593</v>
+      </c>
+      <c r="S184">
+        <v>0.01785954075466623</v>
+      </c>
+      <c r="T184">
+        <v>-0.03531847277429978</v>
+      </c>
+      <c r="U184">
+        <v>0.1042515898544389</v>
+      </c>
+      <c r="V184">
+        <v>-0.003889718695543887</v>
+      </c>
+      <c r="W184">
+        <v>20676.34285714286</v>
+      </c>
+      <c r="X184">
+        <v>21084.04285714286</v>
+      </c>
+      <c r="Y184">
+        <v>19987.54285714286</v>
+      </c>
+      <c r="Z184">
+        <v>20392.44285714286</v>
+      </c>
+      <c r="AA184">
+        <v>3812.225850602857</v>
+      </c>
+      <c r="AB184">
+        <v>25248.57142857143</v>
+      </c>
+      <c r="AC184">
+        <v>0.001344037903738493</v>
+      </c>
+      <c r="AD184">
+        <v>-0.007150253787441004</v>
+      </c>
+      <c r="AE184">
+        <v>-0.008892468126501398</v>
+      </c>
+      <c r="AF184">
+        <v>-0.007811547163895839</v>
+      </c>
+      <c r="AG184">
+        <v>0.168441897395363</v>
+      </c>
+      <c r="AH184">
+        <v>0.04685013481741491</v>
+      </c>
+      <c r="AI184">
+        <v>20560.5</v>
+      </c>
+      <c r="AJ184">
+        <v>21012.635</v>
+      </c>
+      <c r="AK184">
+        <v>26331.958</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>